<commit_message>
replaces '*' with all periods
</commit_message>
<xml_diff>
--- a/IO/input.xlsx
+++ b/IO/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="students"/>
@@ -864,19 +864,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -938,7 +932,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -949,23 +943,26 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1275,28 +1272,28 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="8.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="70.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="8.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="70.7192857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1310,7 +1307,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>132</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1324,7 +1321,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="4" t="s">
         <v>135</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -1338,7 +1335,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>138</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1352,7 +1349,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1366,7 +1363,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="4" t="s">
         <v>146</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1380,7 +1377,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>149</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1394,7 +1391,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>152</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1408,7 +1405,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>156</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -1422,7 +1419,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="4" t="s">
         <v>160</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -1436,7 +1433,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>163</v>
       </c>
       <c r="B12" s="3" t="s">
@@ -1445,12 +1442,12 @@
       <c r="C12" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>137</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="7" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="3" t="s">
@@ -1459,12 +1456,12 @@
       <c r="C13" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>137</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="4" t="s">
         <v>169</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1478,7 +1475,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>172</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -1492,7 +1489,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="4" t="s">
         <v>175</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -1506,7 +1503,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="4" t="s">
         <v>178</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -1520,7 +1517,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="4" t="s">
         <v>181</v>
       </c>
       <c r="B18" s="3" t="s">
@@ -1534,7 +1531,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>184</v>
       </c>
       <c r="B19" s="3" t="s">
@@ -1548,7 +1545,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="4" t="s">
         <v>187</v>
       </c>
       <c r="B20" s="3" t="s">
@@ -1562,7 +1559,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="4" t="s">
         <v>190</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -1576,7 +1573,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="4" t="s">
         <v>193</v>
       </c>
       <c r="B22" s="3" t="s">
@@ -1590,7 +1587,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>196</v>
       </c>
       <c r="B23" s="3" t="s">
@@ -1604,7 +1601,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="7" t="s">
         <v>199</v>
       </c>
       <c r="B24" s="3" t="s">
@@ -1618,7 +1615,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="7" t="s">
         <v>202</v>
       </c>
       <c r="B25" s="3" t="s">
@@ -1632,7 +1629,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>205</v>
       </c>
       <c r="B26" s="3" t="s">
@@ -1646,7 +1643,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>208</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1660,7 +1657,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="4" t="s">
         <v>210</v>
       </c>
       <c r="B28" s="3" t="s">
@@ -1674,7 +1671,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>213</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1688,7 +1685,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="4" t="s">
         <v>216</v>
       </c>
       <c r="B30" s="3" t="s">
@@ -1702,7 +1699,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3" t="s">
+      <c r="A31" s="4" t="s">
         <v>218</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1716,7 +1713,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3" t="s">
+      <c r="A32" s="4" t="s">
         <v>221</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -1730,7 +1727,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="4" t="s">
         <v>224</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1744,7 +1741,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3" t="s">
+      <c r="A34" s="4" t="s">
         <v>227</v>
       </c>
       <c r="B34" s="3" t="s">
@@ -1758,7 +1755,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>230</v>
       </c>
       <c r="B35" s="3" t="s">
@@ -1772,7 +1769,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="7" t="s">
         <v>233</v>
       </c>
       <c r="B36" s="3" t="s">
@@ -1786,7 +1783,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="6" t="s">
+      <c r="A37" s="7" t="s">
         <v>236</v>
       </c>
       <c r="B37" s="3" t="s">
@@ -1800,7 +1797,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>239</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -1814,7 +1811,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="3" t="s">
+      <c r="A39" s="4" t="s">
         <v>242</v>
       </c>
       <c r="B39" s="3" t="s">
@@ -1828,7 +1825,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="4" t="s">
         <v>245</v>
       </c>
       <c r="B40" s="3" t="s">
@@ -1842,7 +1839,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>248</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -1856,7 +1853,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="4" t="s">
         <v>250</v>
       </c>
       <c r="B42" s="3" t="s">
@@ -1870,7 +1867,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="4" t="s">
         <v>253</v>
       </c>
       <c r="B43" s="3" t="s">
@@ -1884,7 +1881,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>256</v>
       </c>
       <c r="B44" s="3" t="s">
@@ -1898,7 +1895,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="3" t="s">
+      <c r="A45" s="4" t="s">
         <v>258</v>
       </c>
       <c r="B45" s="3" t="s">
@@ -1912,7 +1909,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="3" t="s">
+      <c r="A46" s="4" t="s">
         <v>261</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -1926,7 +1923,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>264</v>
       </c>
       <c r="B47" s="3" t="s">
@@ -1940,7 +1937,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="7" t="s">
         <v>267</v>
       </c>
       <c r="B48" s="3" t="s">
@@ -1954,7 +1951,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="7" t="s">
         <v>270</v>
       </c>
       <c r="B49" s="3" t="s">
@@ -1968,7 +1965,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="3" t="s">
+      <c r="A50" s="4" t="s">
         <v>273</v>
       </c>
       <c r="B50" s="3" t="s">
@@ -1982,7 +1979,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="7" t="s">
         <v>275</v>
       </c>
       <c r="B51" s="3" t="s">
@@ -1996,7 +1993,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="7" t="s">
         <v>278</v>
       </c>
       <c r="B52" s="3" t="s">
@@ -2021,16 +2018,16 @@
   </sheetPr>
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="12.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="11.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="51.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="28.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="27.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="12.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="8" width="51.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="28.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="8" width="27.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2225,7 +2222,7 @@
       <c r="C11" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E11" s="3" t="s">
@@ -2261,7 +2258,7 @@
       <c r="C13" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>122</v>
       </c>
       <c r="E13" s="3" t="s">
@@ -2299,19 +2296,19 @@
   </sheetPr>
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="11.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="33.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="31.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="24.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="8" width="13.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="17.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="8" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="11.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="33.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="25.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="31.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="8" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="10" width="13.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="10" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="10" width="25.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2353,22 +2350,22 @@
       <c r="C2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>41</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="5">
         <v>6</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="5">
         <v>12</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="5">
         <v>2</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2382,22 +2379,22 @@
       <c r="C3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="5">
         <v>1</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="5">
         <v>12</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="5">
         <v>2</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2405,28 +2402,28 @@
       <c r="A4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>50</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="5">
         <v>6</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="5">
         <v>12</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="5">
         <v>2</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2434,28 +2431,28 @@
       <c r="A5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>52</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>6</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="5">
         <v>12</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="5">
         <v>2</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2463,28 +2460,28 @@
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="7" t="s">
         <v>54</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>6</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="5">
         <v>12</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="5">
         <v>2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2492,28 +2489,28 @@
       <c r="A7" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>57</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="5">
         <v>6</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="5">
         <v>12</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="5">
         <v>2</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2521,28 +2518,28 @@
       <c r="A8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="5">
         <v>6</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="5">
         <v>12</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="5">
         <v>2</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2550,57 +2547,57 @@
       <c r="A9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="5">
         <v>6</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="5">
         <v>12</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="5">
         <v>2</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="5">
         <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="5">
         <v>1</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="5">
         <v>12</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="5">
         <v>2</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2608,28 +2605,28 @@
       <c r="A11" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="5">
         <v>1</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="5">
         <v>12</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="5">
         <v>2</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2637,28 +2634,28 @@
       <c r="A12" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="7" t="s">
         <v>68</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="5">
         <v>6</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="5">
         <v>12</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="5">
         <v>2</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="5">
         <v>10</v>
       </c>
     </row>
@@ -2672,22 +2669,22 @@
       <c r="C13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>46</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="5">
         <v>1</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="5">
         <v>20</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="5">
         <v>3</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="5">
         <v>15</v>
       </c>
     </row>
@@ -2707,9 +2704,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="38.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="26.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="38.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="10" width="26.433571428571426" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2727,10 +2724,10 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="5">
         <v>24</v>
       </c>
     </row>
@@ -2738,10 +2735,10 @@
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="5">
         <v>12</v>
       </c>
     </row>
@@ -2749,10 +2746,10 @@
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2760,10 +2757,10 @@
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2771,10 +2768,10 @@
       <c r="A6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="5">
         <v>24</v>
       </c>
     </row>
@@ -2782,10 +2779,10 @@
       <c r="A7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="5">
         <v>24</v>
       </c>
     </row>
@@ -2793,10 +2790,10 @@
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2804,10 +2801,10 @@
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2815,10 +2812,10 @@
       <c r="A10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2826,10 +2823,10 @@
       <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="5">
         <v>12</v>
       </c>
     </row>
@@ -2837,10 +2834,10 @@
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="5">
         <v>20</v>
       </c>
     </row>
@@ -2848,10 +2845,10 @@
       <c r="A13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="5">
         <v>24</v>
       </c>
     </row>
@@ -2859,10 +2856,10 @@
       <c r="A14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="5">
         <v>28</v>
       </c>
     </row>
@@ -2870,10 +2867,10 @@
       <c r="A15" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="5">
         <v>28</v>
       </c>
     </row>

</xml_diff>